<commit_message>
Notes on Meeting and Strategy Test
1. revise the notes based on the meeting.
2. test the strategy using some A stock data.  The mean reversion property is not there.
</commit_message>
<xml_diff>
--- a/crypto factor model/whitepaper_feature_extraction.xlsx
+++ b/crypto factor model/whitepaper_feature_extraction.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sunnyyang/Desktop/项目/Cryptocurrency/crypto factor model/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sunny\Desktop\项目\Cryptocurrency\crypto factor model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5C180DE-D461-624A-8F0B-80AE05B8E689}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3E4AFE9-7FA7-43AA-9272-A948713D5CA1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="460" windowWidth="28240" windowHeight="17040" xr2:uid="{A6172E19-C21D-E943-8136-6EFAD0F87F2C}"/>
+    <workbookView xWindow="2328" yWindow="1368" windowWidth="17280" windowHeight="8964" xr2:uid="{A6172E19-C21D-E943-8136-6EFAD0F87F2C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -188,7 +188,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -551,21 +551,21 @@
   <dimension ref="A1:P11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="10.83203125" style="1"/>
-    <col min="4" max="4" width="31.1640625" customWidth="1"/>
-    <col min="5" max="5" width="25.6640625" customWidth="1"/>
-    <col min="6" max="6" width="28.33203125" customWidth="1"/>
-    <col min="7" max="7" width="57.5" customWidth="1"/>
-    <col min="8" max="8" width="40.1640625" customWidth="1"/>
+    <col min="1" max="3" width="10.81640625" style="1"/>
+    <col min="4" max="4" width="31.1796875" customWidth="1"/>
+    <col min="5" max="5" width="25.6328125" customWidth="1"/>
+    <col min="6" max="6" width="28.36328125" customWidth="1"/>
+    <col min="7" max="7" width="57.453125" customWidth="1"/>
+    <col min="8" max="8" width="40.1796875" customWidth="1"/>
     <col min="10" max="10" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -615,7 +615,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -635,7 +635,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -658,7 +658,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -666,7 +666,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
@@ -674,7 +674,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -682,7 +682,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -690,7 +690,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -698,7 +698,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -706,7 +706,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -714,7 +714,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -725,6 +725,7 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -736,9 +737,9 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>18</v>
       </c>

</xml_diff>